<commit_message>
update resign case logic
</commit_message>
<xml_diff>
--- a/python/app/data/test_salary.xlsx
+++ b/python/app/data/test_salary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="19620" windowHeight="12330"/>
+    <workbookView windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1100,8 +1100,8 @@
   </sheetPr>
   <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -2231,12 +2231,8 @@
         <f t="shared" ref="C67:C79" si="4">C66+1</f>
         <v>45475.375</v>
       </c>
-      <c r="D67" s="20">
-        <v>45475.375</v>
-      </c>
-      <c r="E67" s="20">
-        <v>45475.7083333333</v>
-      </c>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20"/>
     </row>
     <row r="68" ht="15" spans="1:5">
       <c r="A68" s="7" t="s">

</xml_diff>